<commit_message>
Update con exchange rate
</commit_message>
<xml_diff>
--- a/Nube/DB.xlsx
+++ b/Nube/DB.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{F3D05FD1-BC23-4066-9565-FC640BBC3E9D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{BF0A6DB5-C106-4E7C-A059-CECC785E4297}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15430" windowHeight="2290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="2220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
+    <sheet name="ResidentialPrices" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:O5"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="51">
   <si>
     <t>Ciudad de mexico</t>
   </si>
@@ -124,6 +125,51 @@
   </si>
   <si>
     <t>Irradiation</t>
+  </si>
+  <si>
+    <t>Tarifa</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Extra consumption</t>
+  </si>
+  <si>
+    <t>First limit</t>
+  </si>
+  <si>
+    <t>Second limit</t>
+  </si>
+  <si>
+    <t>Thrid limit</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
   </si>
 </sst>
 </file>
@@ -266,7 +312,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,6 +490,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -607,7 +659,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
@@ -966,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -982,6 +1037,9 @@
       <c r="C1" t="s">
         <v>35</v>
       </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -993,6 +1051,9 @@
       <c r="C2">
         <v>1834</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -1004,6 +1065,9 @@
       <c r="C3">
         <v>1834</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1015,6 +1079,9 @@
       <c r="C4">
         <v>1834</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -1026,6 +1093,9 @@
       <c r="C5">
         <v>1834</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -1037,6 +1107,9 @@
       <c r="C6">
         <v>1834</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -1048,6 +1121,9 @@
       <c r="C7">
         <v>1834</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1059,6 +1135,9 @@
       <c r="C8">
         <v>1834</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1070,6 +1149,9 @@
       <c r="C9">
         <v>1834</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1081,6 +1163,9 @@
       <c r="C10">
         <v>1834</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1092,6 +1177,9 @@
       <c r="C11">
         <v>1834</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -1103,6 +1191,9 @@
       <c r="C12">
         <v>1834</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -1114,6 +1205,9 @@
       <c r="C13">
         <v>1834</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -1125,6 +1219,9 @@
       <c r="C14">
         <v>1834</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -1136,6 +1233,9 @@
       <c r="C15">
         <v>1834</v>
       </c>
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -1147,8 +1247,11 @@
       <c r="C16">
         <v>1834</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1158,8 +1261,11 @@
       <c r="C17">
         <v>1834</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1169,8 +1275,11 @@
       <c r="C18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1180,8 +1289,11 @@
       <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1191,8 +1303,11 @@
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1202,8 +1317,11 @@
       <c r="C21">
         <v>1921</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1213,8 +1331,11 @@
       <c r="C22">
         <v>1966</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1224,8 +1345,11 @@
       <c r="C23">
         <v>1966</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1235,8 +1359,11 @@
       <c r="C24">
         <v>1861</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1246,8 +1373,11 @@
       <c r="C25">
         <v>1614</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1257,8 +1387,11 @@
       <c r="C26">
         <v>1681</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1268,8 +1401,11 @@
       <c r="C27">
         <v>1681</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1279,8 +1415,11 @@
       <c r="C28">
         <v>1681</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1290,8 +1429,11 @@
       <c r="C29">
         <v>1753</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1301,8 +1443,11 @@
       <c r="C30">
         <v>1677</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1312,8 +1457,11 @@
       <c r="C31">
         <v>1677</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1323,8 +1471,11 @@
       <c r="C32">
         <v>1928</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1334,8 +1485,11 @@
       <c r="C33">
         <v>1928</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1345,8 +1499,11 @@
       <c r="C34">
         <v>1928</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1356,8 +1513,11 @@
       <c r="C35">
         <v>1936</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1367,8 +1527,11 @@
       <c r="C36">
         <v>1936</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1378,8 +1541,11 @@
       <c r="C37">
         <v>1876</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1389,8 +1555,11 @@
       <c r="C38">
         <v>1876</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1400,8 +1569,11 @@
       <c r="C39">
         <v>1876</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1411,8 +1583,11 @@
       <c r="C40">
         <v>1710</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1422,8 +1597,11 @@
       <c r="C41">
         <v>1710</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1433,8 +1611,11 @@
       <c r="C42">
         <v>1710</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1444,8 +1625,11 @@
       <c r="C43">
         <v>1881</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1455,8 +1639,11 @@
       <c r="C44">
         <v>1881</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1466,8 +1653,11 @@
       <c r="C45">
         <v>1858</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1477,8 +1667,11 @@
       <c r="C46">
         <v>1858</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1488,8 +1681,11 @@
       <c r="C47">
         <v>1858</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1499,8 +1695,11 @@
       <c r="C48">
         <v>1858</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1510,8 +1709,11 @@
       <c r="C49">
         <v>1858</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1521,8 +1723,11 @@
       <c r="C50">
         <v>1858</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1532,8 +1737,11 @@
       <c r="C51">
         <v>1892</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D51" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1543,8 +1751,11 @@
       <c r="C52">
         <v>1892</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D52" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1554,8 +1765,11 @@
       <c r="C53">
         <v>1892</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D53" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1565,8 +1779,11 @@
       <c r="C54">
         <v>1892</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D54" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1576,8 +1793,11 @@
       <c r="C55">
         <v>1892</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D55" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1587,8 +1807,11 @@
       <c r="C56">
         <v>1892</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D56" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1598,8 +1821,11 @@
       <c r="C57">
         <v>1892</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D57" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1609,8 +1835,11 @@
       <c r="C58">
         <v>1892</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D58" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1620,8 +1849,11 @@
       <c r="C59">
         <v>1670</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D59" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1631,8 +1863,11 @@
       <c r="C60">
         <v>1670</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D60" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1642,8 +1877,11 @@
       <c r="C61">
         <v>1670</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D61" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1653,8 +1891,11 @@
       <c r="C62">
         <v>1670</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D62" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1664,8 +1905,11 @@
       <c r="C63">
         <v>1876</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D63" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1675,8 +1919,11 @@
       <c r="C64">
         <v>1720</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D64" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1686,8 +1933,11 @@
       <c r="C65">
         <v>1549</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D65" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1697,8 +1947,11 @@
       <c r="C66">
         <v>1549</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D66" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1708,8 +1961,11 @@
       <c r="C67">
         <v>1549</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D67" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1719,8 +1975,11 @@
       <c r="C68">
         <v>1549</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D68" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1730,8 +1989,11 @@
       <c r="C69">
         <v>1867</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D69" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1741,8 +2003,11 @@
       <c r="C70">
         <v>1867</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D70" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1752,8 +2017,11 @@
       <c r="C71">
         <v>1867</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D71" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1763,8 +2031,11 @@
       <c r="C72">
         <v>1867</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D72" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1774,8 +2045,11 @@
       <c r="C73">
         <v>1926</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D73" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1785,8 +2059,11 @@
       <c r="C74">
         <v>1926</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D74" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1796,8 +2073,11 @@
       <c r="C75">
         <v>1926</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D75" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1807,8 +2087,11 @@
       <c r="C76">
         <v>1926</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D76" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1818,8 +2101,11 @@
       <c r="C77">
         <v>1890</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D77" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1829,8 +2115,11 @@
       <c r="C78">
         <v>1555</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D78" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1840,8 +2129,11 @@
       <c r="C79">
         <v>1835</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D79" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1851,8 +2143,11 @@
       <c r="C80">
         <v>1835</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D80" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1862,8 +2157,11 @@
       <c r="C81">
         <v>1756</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D81" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1873,8 +2171,11 @@
       <c r="C82">
         <v>1756</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D82" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1884,8 +2185,11 @@
       <c r="C83">
         <v>1756</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D83" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1895,8 +2199,11 @@
       <c r="C84">
         <v>1863</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D84" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1906,8 +2213,11 @@
       <c r="C85">
         <v>1863</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D85" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1917,8 +2227,11 @@
       <c r="C86">
         <v>1863</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D86" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1928,8 +2241,11 @@
       <c r="C87">
         <v>1516</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D87" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1939,8 +2255,11 @@
       <c r="C88">
         <v>1543</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D88" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1950,8 +2269,11 @@
       <c r="C89">
         <v>1543</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D89" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -1961,8 +2283,11 @@
       <c r="C90">
         <v>1543</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D90" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -1972,8 +2297,11 @@
       <c r="C91">
         <v>1915</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D91" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -1983,8 +2311,11 @@
       <c r="C92">
         <v>1576</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D92" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -1994,8 +2325,11 @@
       <c r="C93">
         <v>1576</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D93" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2005,8 +2339,11 @@
       <c r="C94">
         <v>1576</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D94" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2016,8 +2353,11 @@
       <c r="C95">
         <v>1576</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D95" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2027,8 +2367,11 @@
       <c r="C96">
         <v>1576</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D96" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2038,8 +2381,11 @@
       <c r="C97">
         <v>1576</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D97" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2049,8 +2395,11 @@
       <c r="C98">
         <v>1592</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D98" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2060,8 +2409,11 @@
       <c r="C99">
         <v>1897</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D99" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2071,8 +2423,11 @@
       <c r="C100">
         <v>1897</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D100" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2082,7 +2437,196 @@
       <c r="C101">
         <v>0</v>
       </c>
-    </row>
+      <c r="D101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FC9E6D-A4B1-4E8E-BD47-D6E96E1AB1D7}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2.802</v>
+      </c>
+      <c r="E2" s="3">
+        <v>75</v>
+      </c>
+      <c r="F2" s="3">
+        <v>65</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2.802</v>
+      </c>
+      <c r="E3" s="3">
+        <v>100</v>
+      </c>
+      <c r="F3" s="3">
+        <v>50</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2.802</v>
+      </c>
+      <c r="E4" s="3">
+        <v>125</v>
+      </c>
+      <c r="F4" s="3">
+        <v>100</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.802</v>
+      </c>
+      <c r="E5" s="3">
+        <v>150</v>
+      </c>
+      <c r="F5" s="3">
+        <v>150</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.802</v>
+      </c>
+      <c r="E6" s="3">
+        <v>175</v>
+      </c>
+      <c r="F6" s="3">
+        <v>212.5</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.2469999999999999</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.802</v>
+      </c>
+      <c r="E7" s="3">
+        <v>300</v>
+      </c>
+      <c r="F7" s="3">
+        <v>300</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.2469999999999999</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.802</v>
+      </c>
+      <c r="E8" s="3">
+        <v>300</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1100</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>